<commit_message>
update multiple status from xlsx done
</commit_message>
<xml_diff>
--- a/twitter_experiments/Twitter_Finalized/sample_excel_files/user_tweets.xlsx
+++ b/twitter_experiments/Twitter_Finalized/sample_excel_files/user_tweets.xlsx
@@ -10,10 +10,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -32,15 +32,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -61,23 +61,18 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -121,29 +116,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -163,99 +142,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>